<commit_message>
this is qa enviroment stage
</commit_message>
<xml_diff>
--- a/New Office Document 1.xlsx
+++ b/New Office Document 1.xlsx
@@ -24,6 +24,9 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>This is my first github homework</t>
+  </si>
+  <si>
+    <t>This is my first git branch work</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -392,6 +395,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>